<commit_message>
includes the dataframe in streamlit
</commit_message>
<xml_diff>
--- a/dummy-actas.xlsx
+++ b/dummy-actas.xlsx
@@ -28,7 +28,7 @@
     <t>actores</t>
   </si>
   <si>
-    <t>unidades académicas</t>
+    <t>unidad</t>
   </si>
   <si>
     <t>extracto</t>
@@ -624,12 +624,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -855,6 +858,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="24.38"/>
+    <col customWidth="1" min="2" max="2" width="9.5"/>
+    <col customWidth="1" min="5" max="5" width="25.88"/>
+    <col customWidth="1" min="6" max="6" width="45.25"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -872,7 +881,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -883,7 +892,7 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>44583.0</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -902,18 +911,18 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -921,18 +930,18 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -940,20 +949,20 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -961,20 +970,20 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -982,22 +991,22 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1005,20 +1014,20 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1026,22 +1035,22 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1049,20 +1058,20 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1070,18 +1079,18 @@
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1089,20 +1098,20 @@
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1110,18 +1119,18 @@
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1129,18 +1138,18 @@
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1148,18 +1157,18 @@
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1167,18 +1176,18 @@
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1186,20 +1195,20 @@
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1207,20 +1216,20 @@
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1228,18 +1237,18 @@
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1247,18 +1256,18 @@
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1266,20 +1275,20 @@
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1287,20 +1296,20 @@
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1308,18 +1317,18 @@
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1327,18 +1336,18 @@
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1346,18 +1355,18 @@
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4" t="s">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1365,18 +1374,18 @@
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="5" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1384,20 +1393,20 @@
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1405,18 +1414,18 @@
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1424,20 +1433,20 @@
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4" t="s">
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1445,16 +1454,16 @@
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1462,16 +1471,16 @@
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4" t="s">
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1479,16 +1488,16 @@
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4" t="s">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1496,16 +1505,16 @@
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1513,18 +1522,18 @@
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4" t="s">
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4" t="s">
+      <c r="F34" s="5"/>
+      <c r="G34" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1532,18 +1541,18 @@
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1551,18 +1560,18 @@
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4" t="s">
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
+      <c r="F36" s="5"/>
+      <c r="G36" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1570,16 +1579,16 @@
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B37" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4" t="s">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1587,18 +1596,18 @@
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="B38" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4" t="s">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1606,18 +1615,18 @@
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B39" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4" t="s">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4" t="s">
+      <c r="F39" s="5"/>
+      <c r="G39" s="5" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1625,20 +1634,20 @@
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B40" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4" t="s">
+      <c r="F40" s="5"/>
+      <c r="G40" s="5" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1646,22 +1655,22 @@
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="2">
-        <v>44583.0</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="B41" s="3">
+        <v>44583.0</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="5" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1669,20 +1678,20 @@
       <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4" t="s">
+      <c r="F42" s="5"/>
+      <c r="G42" s="5" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1690,22 +1699,22 @@
       <c r="A43" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="5" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1713,20 +1722,20 @@
       <c r="A44" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
+      <c r="F44" s="5"/>
+      <c r="G44" s="5" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1734,22 +1743,22 @@
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G45" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1757,22 +1766,22 @@
       <c r="A46" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1780,20 +1789,20 @@
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4" t="s">
+      <c r="D47" s="5"/>
+      <c r="E47" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G47" s="5" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1801,20 +1810,20 @@
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4" t="s">
+      <c r="D48" s="5"/>
+      <c r="E48" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G48" s="5" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1822,18 +1831,18 @@
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4" t="s">
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G49" s="5" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1841,22 +1850,22 @@
       <c r="A50" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="G50" s="5" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1864,20 +1873,20 @@
       <c r="A51" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4" t="s">
+      <c r="D51" s="5"/>
+      <c r="E51" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F51" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="G51" s="5" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1885,20 +1894,20 @@
       <c r="A52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4" t="s">
+      <c r="E52" s="5"/>
+      <c r="F52" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="G52" s="5" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1906,18 +1915,18 @@
       <c r="A53" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="3">
         <v>44595.0</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4" t="s">
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="G53" s="5" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>